<commit_message>
added a few sentences to abstract
</commit_message>
<xml_diff>
--- a/docs/proposals/NSF/budgets/budget.xlsx
+++ b/docs/proposals/NSF/budgets/budget.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bquaife/Library/Containers/com.apple.mail/Data/Library/Mail Downloads/9DC0EB7A-8765-44B1-BB4E-D2021BAA7BBC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bquaife/projects/erosion/docs/proposals/NSF/budgets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0224D7E3-19B7-3544-8BDB-A8310AACFD67}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE9546FB-6A8D-5F4C-943F-440C178CDB2D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1840" yWindow="460" windowWidth="26320" windowHeight="19040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24960" yWindow="460" windowWidth="26320" windowHeight="19040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="budg 1" sheetId="4" r:id="rId1"/>
@@ -959,8 +959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -1124,16 +1124,16 @@
         <v>1800.2876279384618</v>
       </c>
       <c r="D8" s="4">
-        <f t="shared" ref="D8:E8" si="1">D7*16.64%</f>
-        <v>1808.6453524480003</v>
+        <f>D7*$I$24</f>
+        <v>1854.2962567766156</v>
       </c>
       <c r="E8" s="4">
-        <f t="shared" si="1"/>
-        <v>931.43015679999996</v>
+        <f>E7*$I$24</f>
+        <v>954.93981220000001</v>
       </c>
       <c r="F8" s="4">
         <f t="shared" si="0"/>
-        <v>4540.3631371864622</v>
+        <v>4609.5236969150774</v>
       </c>
       <c r="H8" s="16" t="s">
         <v>15</v>
@@ -1188,7 +1188,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="4">
-        <f t="shared" ref="E10" si="2">E9*16.64%</f>
+        <f t="shared" ref="E10" si="1">E9*16.64%</f>
         <v>0</v>
       </c>
       <c r="F10" s="4">
@@ -1199,7 +1199,7 @@
         <v>18</v>
       </c>
       <c r="I10" s="13">
-        <v>1920</v>
+        <v>1965</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -1237,11 +1237,11 @@
         <v>0</v>
       </c>
       <c r="D12" s="4">
-        <f t="shared" ref="D12:E12" si="3">D11*$I$18</f>
+        <f t="shared" ref="D12:E12" si="2">D11*$I$18</f>
         <v>0</v>
       </c>
       <c r="E12" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F12" s="4">
@@ -1294,19 +1294,19 @@
       </c>
       <c r="C14" s="4">
         <f>(C13*$I$11) + ($I$5*$I$10)</f>
-        <v>1941</v>
+        <v>1986</v>
       </c>
       <c r="D14" s="4">
         <f>(D13*$I$11) + ($I$5*$I$10)</f>
-        <v>1941.63</v>
+        <v>1986.63</v>
       </c>
       <c r="E14" s="4">
         <f>(E13*$I$11) + ($I$5*$I$10)</f>
-        <v>1942.2789</v>
+        <v>1987.2789</v>
       </c>
       <c r="F14" s="4">
         <f t="shared" si="0"/>
-        <v>5824.9089000000004</v>
+        <v>5959.9089000000004</v>
       </c>
       <c r="H14" s="10"/>
       <c r="I14" s="11"/>
@@ -1382,11 +1382,11 @@
         <v>41272.858974358976</v>
       </c>
       <c r="D18" s="3">
-        <f t="shared" ref="C18:D19" si="4">D5+D7+D9+D11+D13+D15</f>
+        <f t="shared" ref="C18:D19" si="3">D5+D7+D9+D11+D13+D15</f>
         <v>42511.044743589744</v>
       </c>
       <c r="E18" s="3">
-        <f t="shared" ref="E18" si="5">E5+E7+E9+E11+E13+E15</f>
+        <f t="shared" ref="E18" si="4">E5+E7+E9+E11+E13+E15</f>
         <v>38188.572262451285</v>
       </c>
       <c r="F18" s="3">
@@ -1406,20 +1406,20 @@
         <v>29</v>
       </c>
       <c r="C19" s="4">
-        <f t="shared" si="4"/>
-        <v>5399.5497410256412</v>
+        <f t="shared" si="3"/>
+        <v>5444.5497410256412</v>
       </c>
       <c r="D19" s="4">
-        <f t="shared" si="4"/>
-        <v>5458.2853289277955</v>
+        <f t="shared" si="3"/>
+        <v>5548.9362332564106</v>
       </c>
       <c r="E19" s="4">
-        <f t="shared" ref="E19" si="6">E6+E8+E10+E12+E14+E16</f>
-        <v>4632.9593325741889</v>
+        <f t="shared" ref="E19" si="5">E6+E8+E10+E12+E14+E16</f>
+        <v>4701.4689879741891</v>
       </c>
       <c r="F19" s="3">
-        <f t="shared" ref="F19:F20" si="7" xml:space="preserve"> SUM(C19:E19)</f>
-        <v>15490.794402527627</v>
+        <f t="shared" ref="F19:F20" si="6" xml:space="preserve"> SUM(C19:E19)</f>
+        <v>15694.954962256241</v>
       </c>
       <c r="H19" s="12" t="s">
         <v>30</v>
@@ -1435,19 +1435,19 @@
       </c>
       <c r="C20" s="3">
         <f>C18+C19</f>
-        <v>46672.408715384619</v>
+        <v>46717.408715384619</v>
       </c>
       <c r="D20" s="3">
         <f>D18+D19</f>
-        <v>47969.330072517536</v>
+        <v>48059.980976846156</v>
       </c>
       <c r="E20" s="3">
         <f>E18+E19</f>
-        <v>42821.531595025474</v>
+        <v>42890.041250425478</v>
       </c>
       <c r="F20" s="3">
-        <f t="shared" si="7"/>
-        <v>137463.27038292761</v>
+        <f t="shared" si="6"/>
+        <v>137667.43094265624</v>
       </c>
       <c r="H20" s="10" t="s">
         <v>7</v>
@@ -1505,7 +1505,7 @@
         <v>3500</v>
       </c>
       <c r="F24" s="3">
-        <f t="shared" ref="F24:F25" si="8" xml:space="preserve"> SUM(C24:E24)</f>
+        <f t="shared" ref="F24:F25" si="7" xml:space="preserve"> SUM(C24:E24)</f>
         <v>7000</v>
       </c>
       <c r="H24" s="31" t="s">
@@ -1530,7 +1530,7 @@
         <v>0</v>
       </c>
       <c r="F25" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H25" s="12" t="s">
@@ -1555,7 +1555,7 @@
         <v>0</v>
       </c>
       <c r="F26" s="3">
-        <f t="shared" ref="F26:F35" si="9" xml:space="preserve"> SUM(C26:E26)</f>
+        <f t="shared" ref="F26:F35" si="8" xml:space="preserve"> SUM(C26:E26)</f>
         <v>3000</v>
       </c>
       <c r="H26" s="10"/>
@@ -1575,7 +1575,7 @@
         <v>0</v>
       </c>
       <c r="F27" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="H27" s="12" t="s">
@@ -1594,15 +1594,15 @@
         <v>3000</v>
       </c>
       <c r="D28" s="3">
-        <f t="shared" ref="D28:E28" si="10">D24+D25+D26+D27</f>
+        <f t="shared" ref="D28:E28" si="9">D24+D25+D26+D27</f>
         <v>3500</v>
       </c>
       <c r="E28" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>3500</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>10000</v>
       </c>
       <c r="H28" s="27" t="s">
@@ -1626,7 +1626,7 @@
         <v>0</v>
       </c>
       <c r="F29" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="H29" s="12" t="s">
@@ -1653,7 +1653,7 @@
         <v>7483.5</v>
       </c>
       <c r="F30" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>22228.659</v>
       </c>
       <c r="H30" s="29" t="s">
@@ -1669,19 +1669,19 @@
       </c>
       <c r="C31" s="3">
         <f>C28+C20+C29+C30</f>
-        <v>57008.308715384621</v>
+        <v>57053.308715384621</v>
       </c>
       <c r="D31" s="3">
         <f>D28+D20+D29+D30</f>
-        <v>58878.589072517534</v>
+        <v>58969.239976846155</v>
       </c>
       <c r="E31" s="3">
         <f>E28+E20+E29+E30</f>
-        <v>53805.031595025474</v>
+        <v>53873.541250425478</v>
       </c>
       <c r="F31" s="3">
-        <f t="shared" si="9"/>
-        <v>169691.92938292763</v>
+        <f t="shared" si="8"/>
+        <v>169896.08994265625</v>
       </c>
       <c r="H31" s="12" t="s">
         <v>30</v>
@@ -1696,19 +1696,19 @@
       </c>
       <c r="C32" s="3">
         <f>C28+C20</f>
-        <v>49672.408715384619</v>
+        <v>49717.408715384619</v>
       </c>
       <c r="D32" s="3">
-        <f t="shared" ref="D32:E32" si="11">D28+D20</f>
-        <v>51469.330072517536</v>
+        <f t="shared" ref="D32:E32" si="10">D28+D20</f>
+        <v>51559.980976846156</v>
       </c>
       <c r="E32" s="3">
-        <f t="shared" si="11"/>
-        <v>46321.531595025474</v>
+        <f t="shared" si="10"/>
+        <v>46390.041250425478</v>
       </c>
       <c r="F32" s="3">
-        <f t="shared" si="9"/>
-        <v>147463.27038292761</v>
+        <f t="shared" si="8"/>
+        <v>147667.43094265624</v>
       </c>
       <c r="H32" s="10"/>
       <c r="I32" s="11"/>
@@ -1721,7 +1721,7 @@
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
       <c r="F33" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G33" s="4"/>
@@ -1738,19 +1738,19 @@
       </c>
       <c r="C34" s="3">
         <f>C32*$I$39</f>
-        <v>26823.100706307698</v>
+        <v>26847.400706307697</v>
       </c>
       <c r="D34" s="3">
-        <f t="shared" ref="D34:E34" si="12">D32*$I$39</f>
-        <v>27793.43823915947</v>
+        <f t="shared" ref="D34:E34" si="11">D32*$I$39</f>
+        <v>27842.389727496928</v>
       </c>
       <c r="E34" s="3">
-        <f t="shared" si="12"/>
-        <v>25013.627061313757</v>
+        <f t="shared" si="11"/>
+        <v>25050.622275229758</v>
       </c>
       <c r="F34" s="3">
-        <f t="shared" si="9"/>
-        <v>79630.166006780928</v>
+        <f t="shared" si="8"/>
+        <v>79740.412709034383</v>
       </c>
       <c r="H34" s="27" t="s">
         <v>26</v>
@@ -1765,19 +1765,19 @@
       </c>
       <c r="C35" s="3">
         <f>C31+C34</f>
-        <v>83831.409421692311</v>
+        <v>83900.709421692314</v>
       </c>
       <c r="D35" s="3">
         <f>D31+D34</f>
-        <v>86672.027311676997</v>
+        <v>86811.629704343082</v>
       </c>
       <c r="E35" s="3">
         <f>E31+E34</f>
-        <v>78818.658656339234</v>
+        <v>78924.16352565524</v>
       </c>
       <c r="F35" s="37">
-        <f t="shared" si="9"/>
-        <v>249322.09538970853</v>
+        <f t="shared" si="8"/>
+        <v>249636.50265169062</v>
       </c>
       <c r="H35" s="12" t="s">
         <v>27</v>

</xml_diff>